<commit_message>
both lsf tasks work
</commit_message>
<xml_diff>
--- a/LSFphonsem/stim/stimLSFphonsem.xlsx
+++ b/LSFphonsem/stim/stimLSFphonsem.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3705" yWindow="0" windowWidth="22995" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="3705" yWindow="0" windowWidth="22995" windowHeight="16440" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="stimLSFphonsem" sheetId="1" r:id="rId1"/>
-    <sheet name="Train1Phono" sheetId="2" r:id="rId2"/>
+    <sheet name="stimLSFphonsemPrac" sheetId="2" r:id="rId2"/>
     <sheet name="Train2Phono" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="432">
   <si>
     <t>trigTimes</t>
   </si>
@@ -1826,7 +1826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B240" sqref="B240"/>
     </sheetView>
   </sheetViews>
@@ -6085,77 +6085,91 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>424</v>
       </c>
-      <c r="C2">
+      <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>425</v>
       </c>
-      <c r="C3">
+      <c r="B3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="C4">
+      <c r="B4">
         <v>1</v>
       </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>427</v>
       </c>
       <c r="E4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F4" t="s">
         <v>426</v>
       </c>
-      <c r="G4" t="s">
-        <v>426</v>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>428</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>429</v>
+      </c>
+      <c r="E5" t="s">
+        <v>430</v>
+      </c>
+      <c r="F5" t="s">
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -6174,7 +6188,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
piloted LSF expes, ready to run
</commit_message>
<xml_diff>
--- a/LSFphonsem/stim/stimLSFphonsem.xlsx
+++ b/LSFphonsem/stim/stimLSFphonsem.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3705" yWindow="0" windowWidth="22995" windowHeight="16440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3800" yWindow="1980" windowWidth="16100" windowHeight="13400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="stimLSFphonsem" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">stimLSFphonsem!$E$1:$E$176</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="435">
   <si>
     <t>trigTimes</t>
   </si>
@@ -872,9 +872,6 @@
     <t>4.805</t>
   </si>
   <si>
-    <t>9.848</t>
-  </si>
-  <si>
     <t>3.841</t>
   </si>
   <si>
@@ -1130,9 +1127,6 @@
     <t>4.472</t>
   </si>
   <si>
-    <t>6.907</t>
-  </si>
-  <si>
     <t>0.935</t>
   </si>
   <si>
@@ -1320,6 +1314,21 @@
   </si>
   <si>
     <t>family</t>
+  </si>
+  <si>
+    <t>1.335</t>
+  </si>
+  <si>
+    <t>10.611</t>
+  </si>
+  <si>
+    <t>4.238</t>
+  </si>
+  <si>
+    <t>6.874</t>
+  </si>
+  <si>
+    <t>5.473</t>
   </si>
 </sst>
 </file>
@@ -1414,14 +1423,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1826,18 +1835,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H267"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B240" sqref="B240"/>
+    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="B228" sqref="B228"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="14.875" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="2" customWidth="1"/>
     <col min="7" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1845,7 +1854,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -1863,7 +1872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1881,16 +1890,16 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1906,7 +1915,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1924,21 +1933,21 @@
         <v>5</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H4" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>282</v>
+        <v>431</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -1949,12 +1958,12 @@
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -1967,21 +1976,21 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="G6" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H6" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -1992,12 +2001,12 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>285</v>
+        <v>383</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -2010,21 +2019,21 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="G8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H8" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -2037,21 +2046,21 @@
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="G9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H9" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -2064,21 +2073,21 @@
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G10" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H10" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -2089,12 +2098,12 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -2107,21 +2116,21 @@
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G12" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H12" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -2132,12 +2141,12 @@
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -2148,12 +2157,12 @@
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -2166,21 +2175,21 @@
         <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="G15" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H15" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -2193,18 +2202,18 @@
         <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="G16" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -2215,12 +2224,12 @@
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -2231,12 +2240,12 @@
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -2247,12 +2256,12 @@
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>296</v>
+        <v>432</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -2265,21 +2274,21 @@
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="G20" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="H20" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -2292,16 +2301,16 @@
         <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="G21" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H21" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -2317,12 +2326,12 @@
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -2333,12 +2342,12 @@
       </c>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -2349,12 +2358,12 @@
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -2365,12 +2374,12 @@
       </c>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -2383,21 +2392,21 @@
         <v>5</v>
       </c>
       <c r="F26" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="G26" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H26" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -2408,12 +2417,12 @@
       </c>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -2426,21 +2435,21 @@
         <v>5</v>
       </c>
       <c r="F28" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="G28" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H28" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -2451,12 +2460,12 @@
       </c>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -2467,12 +2476,12 @@
       </c>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -2483,12 +2492,12 @@
       </c>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -2499,12 +2508,12 @@
       </c>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -2515,12 +2524,12 @@
       </c>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -2531,12 +2540,12 @@
       </c>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>46</v>
       </c>
       <c r="B35" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
@@ -2547,12 +2556,12 @@
       </c>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
@@ -2563,12 +2572,12 @@
       </c>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
@@ -2579,12 +2588,12 @@
       </c>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
@@ -2595,12 +2604,12 @@
       </c>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
@@ -2611,12 +2620,12 @@
       </c>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>51</v>
       </c>
       <c r="B40" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
@@ -2627,12 +2636,12 @@
       </c>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
@@ -2643,12 +2652,12 @@
       </c>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
@@ -2659,12 +2668,12 @@
       </c>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
@@ -2675,12 +2684,12 @@
       </c>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
@@ -2691,12 +2700,12 @@
       </c>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
@@ -2709,21 +2718,21 @@
         <v>5</v>
       </c>
       <c r="F45" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G45" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H45" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
@@ -2734,12 +2743,12 @@
       </c>
       <c r="E46" s="3"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
@@ -2750,12 +2759,12 @@
       </c>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>59</v>
       </c>
       <c r="B48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
@@ -2766,12 +2775,12 @@
       </c>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>60</v>
       </c>
       <c r="B49" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
@@ -2782,7 +2791,7 @@
       </c>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -2798,12 +2807,12 @@
       </c>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>62</v>
       </c>
       <c r="B51" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="0"/>
@@ -2814,12 +2823,12 @@
       </c>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="0"/>
@@ -2832,21 +2841,21 @@
         <v>5</v>
       </c>
       <c r="F52" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G52" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H52" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
@@ -2857,12 +2866,12 @@
       </c>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>65</v>
       </c>
       <c r="B54" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
@@ -2873,12 +2882,12 @@
       </c>
       <c r="E54" s="3"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>66</v>
       </c>
       <c r="B55" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
@@ -2889,12 +2898,12 @@
       </c>
       <c r="E55" s="3"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
@@ -2904,12 +2913,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>68</v>
       </c>
       <c r="B57" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
@@ -2919,12 +2928,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>69</v>
       </c>
       <c r="B58" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
@@ -2934,12 +2943,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>70</v>
       </c>
       <c r="B59" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="0"/>
@@ -2949,12 +2958,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>71</v>
       </c>
       <c r="B60" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="0"/>
@@ -2964,12 +2973,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>72</v>
       </c>
       <c r="B61" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="0"/>
@@ -2979,12 +2988,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>73</v>
       </c>
       <c r="B62" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="0"/>
@@ -2994,12 +3003,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>74</v>
       </c>
       <c r="B63" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="0"/>
@@ -3009,12 +3018,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>75</v>
       </c>
       <c r="B64" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="0"/>
@@ -3024,12 +3033,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>76</v>
       </c>
       <c r="B65" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="0"/>
@@ -3039,12 +3048,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>77</v>
       </c>
       <c r="B66" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="0"/>
@@ -3054,12 +3063,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>78</v>
       </c>
       <c r="B67" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" ref="C67:C130" si="1">RIGHT(A67,2)</f>
@@ -3069,12 +3078,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>79</v>
       </c>
       <c r="B68" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="1"/>
@@ -3084,12 +3093,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>80</v>
       </c>
       <c r="B69" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="1"/>
@@ -3099,12 +3108,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>81</v>
       </c>
       <c r="B70" t="s">
-        <v>335</v>
+        <v>430</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="1"/>
@@ -3114,12 +3123,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>82</v>
       </c>
       <c r="B71" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
@@ -3129,12 +3138,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
         <v>83</v>
       </c>
       <c r="B72" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
@@ -3144,12 +3153,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" t="s">
         <v>84</v>
       </c>
       <c r="B73" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
@@ -3159,12 +3168,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>85</v>
       </c>
       <c r="B74" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="1"/>
@@ -3174,12 +3183,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>86</v>
       </c>
       <c r="B75" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="1"/>
@@ -3191,12 +3200,12 @@
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
         <v>87</v>
       </c>
       <c r="B76" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
@@ -3206,12 +3215,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
         <v>88</v>
       </c>
       <c r="B77" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
@@ -3221,12 +3230,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>89</v>
       </c>
       <c r="B78" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="1"/>
@@ -3236,12 +3245,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>90</v>
       </c>
       <c r="B79" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="1"/>
@@ -3251,12 +3260,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>91</v>
       </c>
       <c r="B80" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="1"/>
@@ -3266,12 +3275,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>92</v>
       </c>
       <c r="B81" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="1"/>
@@ -3281,12 +3290,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
         <v>93</v>
       </c>
       <c r="B82" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="1"/>
@@ -3296,12 +3305,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
         <v>94</v>
       </c>
       <c r="B83" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="1"/>
@@ -3311,12 +3320,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
         <v>95</v>
       </c>
       <c r="B84" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="1"/>
@@ -3326,12 +3335,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>96</v>
       </c>
       <c r="B85" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="1"/>
@@ -3341,12 +3350,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
         <v>97</v>
       </c>
       <c r="B86" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="1"/>
@@ -3356,12 +3365,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
         <v>98</v>
       </c>
       <c r="B87" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="1"/>
@@ -3371,12 +3380,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
         <v>99</v>
       </c>
       <c r="B88" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="1"/>
@@ -3386,12 +3395,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
         <v>100</v>
       </c>
       <c r="B89" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="1"/>
@@ -3401,12 +3410,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
         <v>101</v>
       </c>
       <c r="B90" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="1"/>
@@ -3416,12 +3425,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
         <v>102</v>
       </c>
       <c r="B91" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="1"/>
@@ -3431,12 +3440,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
         <v>103</v>
       </c>
       <c r="B92" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="1"/>
@@ -3446,12 +3455,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
         <v>104</v>
       </c>
       <c r="B93" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="1"/>
@@ -3461,12 +3470,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
         <v>105</v>
       </c>
       <c r="B94" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="1"/>
@@ -3476,12 +3485,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95" t="s">
         <v>106</v>
       </c>
       <c r="B95" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="1"/>
@@ -3491,12 +3500,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
         <v>107</v>
       </c>
       <c r="B96" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="1"/>
@@ -3506,12 +3515,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>108</v>
       </c>
       <c r="B97" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="1"/>
@@ -3521,12 +3530,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>109</v>
       </c>
       <c r="B98" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="1"/>
@@ -3536,12 +3545,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>110</v>
       </c>
       <c r="B99" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="1"/>
@@ -3551,12 +3560,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>111</v>
       </c>
       <c r="B100" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="1"/>
@@ -3566,12 +3575,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>112</v>
       </c>
       <c r="B101" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="1"/>
@@ -3581,12 +3590,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>113</v>
       </c>
       <c r="B102" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="1"/>
@@ -3596,12 +3605,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
         <v>114</v>
       </c>
       <c r="B103" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="1"/>
@@ -3611,12 +3620,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>115</v>
       </c>
       <c r="B104" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="1"/>
@@ -3626,12 +3635,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>116</v>
       </c>
       <c r="B105" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="1"/>
@@ -3641,12 +3650,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
         <v>117</v>
       </c>
       <c r="B106" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C106" t="str">
         <f t="shared" si="1"/>
@@ -3656,12 +3665,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
         <v>118</v>
       </c>
       <c r="B107" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C107" t="str">
         <f t="shared" si="1"/>
@@ -3671,12 +3680,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
         <v>119</v>
       </c>
       <c r="B108" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C108" t="str">
         <f t="shared" si="1"/>
@@ -3686,12 +3695,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
         <v>120</v>
       </c>
       <c r="B109" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C109" t="str">
         <f t="shared" si="1"/>
@@ -3701,12 +3710,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
         <v>121</v>
       </c>
       <c r="B110" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C110" t="str">
         <f t="shared" si="1"/>
@@ -3716,12 +3725,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
         <v>122</v>
       </c>
       <c r="B111" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C111" t="str">
         <f t="shared" si="1"/>
@@ -3731,12 +3740,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
         <v>123</v>
       </c>
       <c r="B112" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C112" t="str">
         <f t="shared" si="1"/>
@@ -3746,12 +3755,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
         <v>124</v>
       </c>
       <c r="B113" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C113" t="str">
         <f t="shared" si="1"/>
@@ -3761,12 +3770,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
         <v>125</v>
       </c>
       <c r="B114" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C114" t="str">
         <f t="shared" si="1"/>
@@ -3776,12 +3785,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
         <v>126</v>
       </c>
       <c r="B115" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C115" t="str">
         <f t="shared" si="1"/>
@@ -3791,12 +3800,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
         <v>127</v>
       </c>
       <c r="B116" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C116" t="str">
         <f t="shared" si="1"/>
@@ -3806,12 +3815,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
         <v>128</v>
       </c>
       <c r="B117" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C117" t="str">
         <f t="shared" si="1"/>
@@ -3821,12 +3830,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4">
       <c r="A118" t="s">
         <v>129</v>
       </c>
       <c r="B118" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C118" t="str">
         <f t="shared" si="1"/>
@@ -3836,12 +3845,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4">
       <c r="A119" t="s">
         <v>130</v>
       </c>
       <c r="B119" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C119" t="str">
         <f t="shared" si="1"/>
@@ -3851,12 +3860,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4">
       <c r="A120" t="s">
         <v>131</v>
       </c>
       <c r="B120" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C120" t="str">
         <f t="shared" si="1"/>
@@ -3866,12 +3875,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4">
       <c r="A121" t="s">
         <v>132</v>
       </c>
       <c r="B121" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C121" t="str">
         <f t="shared" si="1"/>
@@ -3881,12 +3890,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4">
       <c r="A122" t="s">
         <v>133</v>
       </c>
       <c r="B122" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C122" t="str">
         <f t="shared" si="1"/>
@@ -3896,12 +3905,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4">
       <c r="A123" t="s">
         <v>134</v>
       </c>
       <c r="B123" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C123" t="str">
         <f t="shared" si="1"/>
@@ -3911,12 +3920,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4">
       <c r="A124" t="s">
         <v>135</v>
       </c>
       <c r="B124" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C124" t="str">
         <f t="shared" si="1"/>
@@ -3926,12 +3935,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4">
       <c r="A125" t="s">
         <v>136</v>
       </c>
       <c r="B125" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C125" t="str">
         <f t="shared" si="1"/>
@@ -3941,12 +3950,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
         <v>137</v>
       </c>
       <c r="B126" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C126" t="str">
         <f t="shared" si="1"/>
@@ -3956,12 +3965,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4">
       <c r="A127" t="s">
         <v>138</v>
       </c>
       <c r="B127" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C127" t="str">
         <f t="shared" si="1"/>
@@ -3971,12 +3980,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4">
       <c r="A128" t="s">
         <v>139</v>
       </c>
       <c r="B128" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C128" t="str">
         <f t="shared" si="1"/>
@@ -3986,12 +3995,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4">
       <c r="A129" t="s">
         <v>140</v>
       </c>
       <c r="B129" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C129" t="str">
         <f t="shared" si="1"/>
@@ -4001,12 +4010,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4">
       <c r="A130" t="s">
         <v>141</v>
       </c>
       <c r="B130" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C130" t="str">
         <f t="shared" si="1"/>
@@ -4016,12 +4025,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4">
       <c r="A131" t="s">
         <v>142</v>
       </c>
       <c r="B131" t="s">
-        <v>368</v>
+        <v>433</v>
       </c>
       <c r="C131" t="str">
         <f t="shared" ref="C131:C194" si="2">RIGHT(A131,2)</f>
@@ -4031,12 +4040,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4">
       <c r="A132" t="s">
         <v>143</v>
       </c>
       <c r="B132" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C132" t="str">
         <f t="shared" si="2"/>
@@ -4046,12 +4055,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4">
       <c r="A133" t="s">
         <v>144</v>
       </c>
       <c r="B133" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C133" t="str">
         <f t="shared" si="2"/>
@@ -4061,12 +4070,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4">
       <c r="A134" t="s">
         <v>145</v>
       </c>
       <c r="B134" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C134" t="str">
         <f t="shared" si="2"/>
@@ -4076,12 +4085,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4">
       <c r="A135" t="s">
         <v>146</v>
       </c>
       <c r="B135" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C135" t="str">
         <f t="shared" si="2"/>
@@ -4091,12 +4100,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4">
       <c r="A136" t="s">
         <v>147</v>
       </c>
       <c r="B136" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C136" t="str">
         <f t="shared" si="2"/>
@@ -4106,12 +4115,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4">
       <c r="A137" t="s">
         <v>148</v>
       </c>
       <c r="B137" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C137" t="str">
         <f t="shared" si="2"/>
@@ -4121,12 +4130,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4">
       <c r="A138" t="s">
         <v>149</v>
       </c>
       <c r="B138" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C138" t="str">
         <f t="shared" si="2"/>
@@ -4136,12 +4145,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4">
       <c r="A139" t="s">
         <v>150</v>
       </c>
       <c r="B139" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C139" t="str">
         <f t="shared" si="2"/>
@@ -4151,12 +4160,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4">
       <c r="A140" t="s">
         <v>151</v>
       </c>
       <c r="B140" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C140" t="str">
         <f t="shared" si="2"/>
@@ -4166,12 +4175,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4">
       <c r="A141" t="s">
         <v>152</v>
       </c>
       <c r="B141" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C141" t="str">
         <f t="shared" si="2"/>
@@ -4181,12 +4190,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4">
       <c r="A142" t="s">
         <v>153</v>
       </c>
       <c r="B142" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C142" t="str">
         <f t="shared" si="2"/>
@@ -4196,12 +4205,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4">
       <c r="A143" t="s">
         <v>154</v>
       </c>
       <c r="B143" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C143" t="str">
         <f t="shared" si="2"/>
@@ -4211,12 +4220,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4">
       <c r="A144" t="s">
         <v>155</v>
       </c>
       <c r="B144" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C144" t="str">
         <f t="shared" si="2"/>
@@ -4226,12 +4235,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4">
       <c r="A145" t="s">
         <v>156</v>
       </c>
       <c r="B145" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C145" t="str">
         <f t="shared" si="2"/>
@@ -4241,12 +4250,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4">
       <c r="A146" t="s">
         <v>157</v>
       </c>
       <c r="B146" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C146" t="str">
         <f t="shared" si="2"/>
@@ -4256,12 +4265,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4">
       <c r="A147" t="s">
         <v>158</v>
       </c>
       <c r="B147" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C147" t="str">
         <f t="shared" si="2"/>
@@ -4271,12 +4280,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4">
       <c r="A148" t="s">
         <v>159</v>
       </c>
       <c r="B148" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C148" t="str">
         <f t="shared" si="2"/>
@@ -4286,12 +4295,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4">
       <c r="A149" t="s">
         <v>160</v>
       </c>
       <c r="B149" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C149" t="str">
         <f t="shared" si="2"/>
@@ -4301,12 +4310,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4">
       <c r="A150" t="s">
         <v>161</v>
       </c>
       <c r="B150" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C150" t="str">
         <f t="shared" si="2"/>
@@ -4316,12 +4325,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4">
       <c r="A151" t="s">
         <v>162</v>
       </c>
       <c r="B151" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C151" t="str">
         <f t="shared" si="2"/>
@@ -4331,12 +4340,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4">
       <c r="A152" t="s">
         <v>163</v>
       </c>
       <c r="B152" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C152" t="str">
         <f t="shared" si="2"/>
@@ -4346,12 +4355,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4">
       <c r="A153" t="s">
         <v>164</v>
       </c>
       <c r="B153" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C153" t="str">
         <f t="shared" si="2"/>
@@ -4361,12 +4370,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4">
       <c r="A154" t="s">
         <v>165</v>
       </c>
       <c r="B154" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C154" t="str">
         <f t="shared" si="2"/>
@@ -4376,12 +4385,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4">
       <c r="A155" t="s">
         <v>166</v>
       </c>
       <c r="B155" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C155" t="str">
         <f t="shared" si="2"/>
@@ -4391,12 +4400,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4">
       <c r="A156" t="s">
         <v>167</v>
       </c>
       <c r="B156" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C156" t="str">
         <f t="shared" si="2"/>
@@ -4406,12 +4415,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4">
       <c r="A157" t="s">
         <v>168</v>
       </c>
       <c r="B157" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C157" t="str">
         <f t="shared" si="2"/>
@@ -4421,12 +4430,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4">
       <c r="A158" t="s">
         <v>169</v>
       </c>
       <c r="B158" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C158" t="str">
         <f t="shared" si="2"/>
@@ -4436,12 +4445,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4">
       <c r="A159" t="s">
         <v>170</v>
       </c>
       <c r="B159" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C159" t="str">
         <f t="shared" si="2"/>
@@ -4451,12 +4460,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4">
       <c r="A160" t="s">
         <v>171</v>
       </c>
       <c r="B160" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C160" t="str">
         <f t="shared" si="2"/>
@@ -4466,12 +4475,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4">
       <c r="A161" t="s">
         <v>172</v>
       </c>
       <c r="B161" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C161" t="str">
         <f t="shared" si="2"/>
@@ -4481,12 +4490,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4">
       <c r="A162" t="s">
         <v>173</v>
       </c>
       <c r="B162" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C162" t="str">
         <f t="shared" si="2"/>
@@ -4496,12 +4505,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4">
       <c r="A163" t="s">
         <v>174</v>
       </c>
       <c r="B163" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C163" t="str">
         <f t="shared" si="2"/>
@@ -4511,12 +4520,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4">
       <c r="A164" t="s">
         <v>175</v>
       </c>
       <c r="B164" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C164" t="str">
         <f t="shared" si="2"/>
@@ -4526,12 +4535,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4">
       <c r="A165" t="s">
         <v>176</v>
       </c>
       <c r="B165" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C165" t="str">
         <f t="shared" si="2"/>
@@ -4541,12 +4550,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4">
       <c r="A166" t="s">
         <v>177</v>
       </c>
       <c r="B166" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C166" t="str">
         <f t="shared" si="2"/>
@@ -4556,12 +4565,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4">
       <c r="A167" t="s">
         <v>178</v>
       </c>
       <c r="B167" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C167" t="str">
         <f t="shared" si="2"/>
@@ -4571,12 +4580,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4">
       <c r="A168" t="s">
         <v>179</v>
       </c>
       <c r="B168" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C168" t="str">
         <f t="shared" si="2"/>
@@ -4586,12 +4595,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4">
       <c r="A169" t="s">
         <v>180</v>
       </c>
       <c r="B169" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C169" t="str">
         <f t="shared" si="2"/>
@@ -4601,12 +4610,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4">
       <c r="A170" t="s">
         <v>181</v>
       </c>
       <c r="B170" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C170" t="str">
         <f t="shared" si="2"/>
@@ -4616,12 +4625,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4">
       <c r="A171" t="s">
         <v>182</v>
       </c>
       <c r="B171" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C171" t="str">
         <f t="shared" si="2"/>
@@ -4631,12 +4640,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4">
       <c r="A172" t="s">
         <v>183</v>
       </c>
       <c r="B172" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C172" t="str">
         <f t="shared" si="2"/>
@@ -4646,12 +4655,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4">
       <c r="A173" t="s">
         <v>184</v>
       </c>
       <c r="B173" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C173" t="str">
         <f t="shared" si="2"/>
@@ -4661,12 +4670,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4">
       <c r="A174" t="s">
         <v>185</v>
       </c>
       <c r="B174" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C174" t="str">
         <f t="shared" si="2"/>
@@ -4676,12 +4685,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4">
       <c r="A175" t="s">
         <v>186</v>
       </c>
       <c r="B175" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C175" t="str">
         <f t="shared" si="2"/>
@@ -4691,12 +4700,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4">
       <c r="A176" t="s">
         <v>187</v>
       </c>
       <c r="B176" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C176" t="str">
         <f t="shared" si="2"/>
@@ -4706,12 +4715,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4">
       <c r="A177" t="s">
         <v>188</v>
       </c>
       <c r="B177" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C177" t="str">
         <f t="shared" si="2"/>
@@ -4721,12 +4730,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4">
       <c r="A178" t="s">
         <v>189</v>
       </c>
       <c r="B178" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C178" t="str">
         <f t="shared" si="2"/>
@@ -4736,12 +4745,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4">
       <c r="A179" t="s">
         <v>190</v>
       </c>
       <c r="B179" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C179" t="str">
         <f t="shared" si="2"/>
@@ -4751,12 +4760,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4">
       <c r="A180" t="s">
         <v>191</v>
       </c>
       <c r="B180" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C180" t="str">
         <f t="shared" si="2"/>
@@ -4766,12 +4775,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4">
       <c r="A181" t="s">
         <v>192</v>
       </c>
       <c r="B181" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C181" t="str">
         <f t="shared" si="2"/>
@@ -4781,12 +4790,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4">
       <c r="A182" t="s">
         <v>193</v>
       </c>
       <c r="B182" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C182" t="str">
         <f t="shared" si="2"/>
@@ -4796,12 +4805,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4">
       <c r="A183" t="s">
         <v>194</v>
       </c>
       <c r="B183" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C183" t="str">
         <f t="shared" si="2"/>
@@ -4811,12 +4820,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4">
       <c r="A184" t="s">
         <v>195</v>
       </c>
       <c r="B184" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C184" t="str">
         <f t="shared" si="2"/>
@@ -4826,12 +4835,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4">
       <c r="A185" t="s">
         <v>196</v>
       </c>
       <c r="B185" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C185" t="str">
         <f t="shared" si="2"/>
@@ -4841,12 +4850,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4">
       <c r="A186" t="s">
         <v>197</v>
       </c>
       <c r="B186" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C186" t="str">
         <f t="shared" si="2"/>
@@ -4856,12 +4865,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4">
       <c r="A187" t="s">
         <v>198</v>
       </c>
       <c r="B187" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C187" t="str">
         <f t="shared" si="2"/>
@@ -4871,12 +4880,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4">
       <c r="A188" t="s">
         <v>199</v>
       </c>
       <c r="B188" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C188" t="str">
         <f t="shared" si="2"/>
@@ -4886,12 +4895,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4">
       <c r="A189" t="s">
         <v>200</v>
       </c>
       <c r="B189" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C189" t="str">
         <f t="shared" si="2"/>
@@ -4901,12 +4910,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4">
       <c r="A190" t="s">
         <v>201</v>
       </c>
       <c r="B190" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C190" t="str">
         <f t="shared" si="2"/>
@@ -4916,12 +4925,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4">
       <c r="A191" t="s">
         <v>202</v>
       </c>
       <c r="B191" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C191" t="str">
         <f t="shared" si="2"/>
@@ -4931,12 +4940,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4">
       <c r="A192" t="s">
         <v>203</v>
       </c>
       <c r="B192" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C192" t="str">
         <f t="shared" si="2"/>
@@ -4946,12 +4955,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4">
       <c r="A193" t="s">
         <v>204</v>
       </c>
       <c r="B193" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C193" t="str">
         <f t="shared" si="2"/>
@@ -4961,12 +4970,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4">
       <c r="A194" t="s">
         <v>205</v>
       </c>
       <c r="B194" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C194" t="str">
         <f t="shared" si="2"/>
@@ -4976,12 +4985,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4">
       <c r="A195" t="s">
         <v>206</v>
       </c>
       <c r="B195" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C195" t="str">
         <f t="shared" ref="C195:C258" si="3">RIGHT(A195,2)</f>
@@ -4991,12 +5000,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4">
       <c r="A196" t="s">
         <v>207</v>
       </c>
       <c r="B196" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C196" t="str">
         <f t="shared" si="3"/>
@@ -5006,12 +5015,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4">
       <c r="A197" t="s">
         <v>208</v>
       </c>
       <c r="B197" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C197" t="str">
         <f t="shared" si="3"/>
@@ -5021,12 +5030,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4">
       <c r="A198" t="s">
         <v>209</v>
       </c>
       <c r="B198" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C198" t="str">
         <f t="shared" si="3"/>
@@ -5036,12 +5045,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4">
       <c r="A199" t="s">
         <v>210</v>
       </c>
       <c r="B199" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C199" t="str">
         <f t="shared" si="3"/>
@@ -5051,12 +5060,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4">
       <c r="A200" t="s">
         <v>211</v>
       </c>
       <c r="B200" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C200" t="str">
         <f t="shared" si="3"/>
@@ -5066,7 +5075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4">
       <c r="A201" t="s">
         <v>212</v>
       </c>
@@ -5081,12 +5090,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4">
       <c r="A202" t="s">
         <v>213</v>
       </c>
       <c r="B202" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C202" t="str">
         <f t="shared" si="3"/>
@@ -5096,12 +5105,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4">
       <c r="A203" t="s">
         <v>214</v>
       </c>
       <c r="B203" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C203" t="str">
         <f t="shared" si="3"/>
@@ -5111,7 +5120,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4">
       <c r="A204" t="s">
         <v>215</v>
       </c>
@@ -5126,12 +5135,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4">
       <c r="A205" t="s">
         <v>216</v>
       </c>
       <c r="B205" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C205" t="str">
         <f t="shared" si="3"/>
@@ -5141,12 +5150,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4">
       <c r="A206" t="s">
         <v>217</v>
       </c>
       <c r="B206" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C206" t="str">
         <f t="shared" si="3"/>
@@ -5156,12 +5165,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4">
       <c r="A207" t="s">
         <v>218</v>
       </c>
       <c r="B207" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C207" t="str">
         <f t="shared" si="3"/>
@@ -5171,12 +5180,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4">
       <c r="A208" t="s">
         <v>219</v>
       </c>
       <c r="B208" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C208" t="str">
         <f t="shared" si="3"/>
@@ -5186,12 +5195,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4">
       <c r="A209" t="s">
         <v>220</v>
       </c>
       <c r="B209" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C209" t="str">
         <f t="shared" si="3"/>
@@ -5201,12 +5210,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4">
       <c r="A210" t="s">
         <v>221</v>
       </c>
       <c r="B210" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C210" t="str">
         <f t="shared" si="3"/>
@@ -5216,12 +5225,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4">
       <c r="A211" t="s">
         <v>222</v>
       </c>
       <c r="B211" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C211" t="str">
         <f t="shared" si="3"/>
@@ -5231,12 +5240,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4">
       <c r="A212" t="s">
         <v>223</v>
       </c>
       <c r="B212" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C212" t="str">
         <f t="shared" si="3"/>
@@ -5246,7 +5255,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4">
       <c r="A213" t="s">
         <v>224</v>
       </c>
@@ -5261,12 +5270,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4">
       <c r="A214" t="s">
         <v>225</v>
       </c>
       <c r="B214" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C214" t="str">
         <f t="shared" si="3"/>
@@ -5276,12 +5285,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4">
       <c r="A215" t="s">
         <v>226</v>
       </c>
       <c r="B215" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C215" t="str">
         <f t="shared" si="3"/>
@@ -5291,12 +5300,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4">
       <c r="A216" t="s">
         <v>227</v>
       </c>
       <c r="B216" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C216" t="str">
         <f t="shared" si="3"/>
@@ -5306,12 +5315,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4">
       <c r="A217" t="s">
         <v>228</v>
       </c>
       <c r="B217" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C217" t="str">
         <f t="shared" si="3"/>
@@ -5321,12 +5330,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4">
       <c r="A218" t="s">
         <v>229</v>
       </c>
       <c r="B218" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C218" t="str">
         <f t="shared" si="3"/>
@@ -5336,12 +5345,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4">
       <c r="A219" t="s">
         <v>230</v>
       </c>
       <c r="B219" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C219" t="str">
         <f t="shared" si="3"/>
@@ -5351,12 +5360,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4">
       <c r="A220" t="s">
         <v>231</v>
       </c>
       <c r="B220" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C220" t="str">
         <f t="shared" si="3"/>
@@ -5366,12 +5375,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4">
       <c r="A221" t="s">
         <v>232</v>
       </c>
       <c r="B221" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C221" t="str">
         <f t="shared" si="3"/>
@@ -5381,12 +5390,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4">
       <c r="A222" t="s">
         <v>233</v>
       </c>
       <c r="B222" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C222" t="str">
         <f t="shared" si="3"/>
@@ -5396,12 +5405,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4">
       <c r="A223" t="s">
         <v>234</v>
       </c>
       <c r="B223" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C223" t="str">
         <f t="shared" si="3"/>
@@ -5411,12 +5420,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4">
       <c r="A224" t="s">
         <v>235</v>
       </c>
       <c r="B224" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C224" t="str">
         <f t="shared" si="3"/>
@@ -5426,12 +5435,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4">
       <c r="A225" t="s">
         <v>236</v>
       </c>
       <c r="B225" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C225" t="str">
         <f t="shared" si="3"/>
@@ -5441,12 +5450,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4">
       <c r="A226" t="s">
         <v>237</v>
       </c>
       <c r="B226" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C226" t="str">
         <f t="shared" si="3"/>
@@ -5456,12 +5465,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4">
       <c r="A227" t="s">
         <v>238</v>
       </c>
       <c r="B227" t="s">
-        <v>387</v>
+        <v>434</v>
       </c>
       <c r="C227" t="str">
         <f t="shared" si="3"/>
@@ -5471,12 +5480,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4">
       <c r="A228" t="s">
         <v>239</v>
       </c>
       <c r="B228" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C228" t="str">
         <f t="shared" si="3"/>
@@ -5486,12 +5495,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4">
       <c r="A229" t="s">
         <v>240</v>
       </c>
       <c r="B229" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C229" t="str">
         <f t="shared" si="3"/>
@@ -5501,12 +5510,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4">
       <c r="A230" t="s">
         <v>241</v>
       </c>
       <c r="B230" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C230" t="str">
         <f t="shared" si="3"/>
@@ -5516,12 +5525,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4">
       <c r="A231" t="s">
         <v>242</v>
       </c>
       <c r="B231" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C231" t="str">
         <f t="shared" si="3"/>
@@ -5531,12 +5540,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4">
       <c r="A232" t="s">
         <v>243</v>
       </c>
       <c r="B232" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C232" t="str">
         <f t="shared" si="3"/>
@@ -5546,12 +5555,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4">
       <c r="A233" t="s">
         <v>244</v>
       </c>
       <c r="B233" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C233" t="str">
         <f t="shared" si="3"/>
@@ -5561,7 +5570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4">
       <c r="A234" t="s">
         <v>245</v>
       </c>
@@ -5576,12 +5585,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4">
       <c r="A235" t="s">
         <v>246</v>
       </c>
       <c r="B235" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C235" t="str">
         <f t="shared" si="3"/>
@@ -5591,12 +5600,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4">
       <c r="A236" t="s">
         <v>247</v>
       </c>
       <c r="B236" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C236" t="str">
         <f t="shared" si="3"/>
@@ -5606,12 +5615,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4">
       <c r="A237" t="s">
         <v>248</v>
       </c>
       <c r="B237" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C237" t="str">
         <f t="shared" si="3"/>
@@ -5621,12 +5630,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4">
       <c r="A238" t="s">
         <v>249</v>
       </c>
       <c r="B238" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C238" t="str">
         <f t="shared" si="3"/>
@@ -5636,12 +5645,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4">
       <c r="A239" t="s">
         <v>250</v>
       </c>
       <c r="B239" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C239" t="str">
         <f t="shared" si="3"/>
@@ -5651,12 +5660,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4">
       <c r="A240" t="s">
         <v>251</v>
       </c>
       <c r="B240" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C240" t="str">
         <f t="shared" si="3"/>
@@ -5666,12 +5675,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4">
       <c r="A241" t="s">
         <v>252</v>
       </c>
       <c r="B241" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C241" t="str">
         <f t="shared" si="3"/>
@@ -5681,12 +5690,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4">
       <c r="A242" t="s">
         <v>253</v>
       </c>
       <c r="B242" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C242" t="str">
         <f t="shared" si="3"/>
@@ -5696,12 +5705,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4">
       <c r="A243" t="s">
         <v>254</v>
       </c>
       <c r="B243" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C243" t="str">
         <f t="shared" si="3"/>
@@ -5711,12 +5720,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4">
       <c r="A244" t="s">
         <v>255</v>
       </c>
       <c r="B244" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C244" t="str">
         <f t="shared" si="3"/>
@@ -5726,12 +5735,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4">
       <c r="A245" t="s">
         <v>256</v>
       </c>
       <c r="B245" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C245" t="str">
         <f t="shared" si="3"/>
@@ -5741,12 +5750,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4">
       <c r="A246" t="s">
         <v>257</v>
       </c>
       <c r="B246" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C246" t="str">
         <f t="shared" si="3"/>
@@ -5756,12 +5765,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4">
       <c r="A247" t="s">
         <v>258</v>
       </c>
       <c r="B247" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C247" t="str">
         <f t="shared" si="3"/>
@@ -5771,12 +5780,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4">
       <c r="A248" t="s">
         <v>259</v>
       </c>
       <c r="B248" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C248" t="str">
         <f t="shared" si="3"/>
@@ -5786,12 +5795,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4">
       <c r="A249" t="s">
         <v>260</v>
       </c>
       <c r="B249" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C249" t="str">
         <f t="shared" si="3"/>
@@ -5801,12 +5810,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4">
       <c r="A250" t="s">
         <v>261</v>
       </c>
       <c r="B250" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C250" t="str">
         <f t="shared" si="3"/>
@@ -5816,12 +5825,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4">
       <c r="A251" t="s">
         <v>262</v>
       </c>
       <c r="B251" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C251" t="str">
         <f t="shared" si="3"/>
@@ -5831,12 +5840,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4">
       <c r="A252" t="s">
         <v>263</v>
       </c>
       <c r="B252" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C252" t="str">
         <f t="shared" si="3"/>
@@ -5846,12 +5855,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4">
       <c r="A253" t="s">
         <v>264</v>
       </c>
       <c r="B253" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C253" t="str">
         <f t="shared" si="3"/>
@@ -5861,12 +5870,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4">
       <c r="A254" t="s">
         <v>265</v>
       </c>
       <c r="B254" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C254" t="str">
         <f t="shared" si="3"/>
@@ -5876,12 +5885,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4">
       <c r="A255" t="s">
         <v>266</v>
       </c>
       <c r="B255" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C255" t="str">
         <f t="shared" si="3"/>
@@ -5891,12 +5900,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4">
       <c r="A256" t="s">
         <v>267</v>
       </c>
       <c r="B256" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C256" t="str">
         <f t="shared" si="3"/>
@@ -5906,12 +5915,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:4">
       <c r="A257" t="s">
         <v>268</v>
       </c>
       <c r="B257" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C257" t="str">
         <f t="shared" si="3"/>
@@ -5921,12 +5930,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:4">
       <c r="A258" t="s">
         <v>269</v>
       </c>
       <c r="B258" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C258" t="str">
         <f t="shared" si="3"/>
@@ -5936,12 +5945,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:4">
       <c r="A259" t="s">
         <v>270</v>
       </c>
       <c r="B259" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C259" t="str">
         <f t="shared" ref="C259:C267" si="4">RIGHT(A259,2)</f>
@@ -5951,12 +5960,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:4">
       <c r="A260" t="s">
         <v>271</v>
       </c>
       <c r="B260" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C260" t="str">
         <f t="shared" si="4"/>
@@ -5966,12 +5975,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:4">
       <c r="A261" t="s">
         <v>272</v>
       </c>
       <c r="B261" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C261" t="str">
         <f t="shared" si="4"/>
@@ -5981,12 +5990,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:4">
       <c r="A262" t="s">
         <v>273</v>
       </c>
       <c r="B262" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C262" t="str">
         <f t="shared" si="4"/>
@@ -5996,12 +6005,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:4">
       <c r="A263" t="s">
         <v>274</v>
       </c>
       <c r="B263" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C263" t="str">
         <f t="shared" si="4"/>
@@ -6011,12 +6020,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:4">
       <c r="A264" t="s">
         <v>275</v>
       </c>
       <c r="B264" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C264" t="str">
         <f t="shared" si="4"/>
@@ -6026,12 +6035,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:4">
       <c r="A265" t="s">
         <v>276</v>
       </c>
       <c r="B265" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C265" t="str">
         <f t="shared" si="4"/>
@@ -6041,12 +6050,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:4">
       <c r="A266" t="s">
         <v>277</v>
       </c>
       <c r="B266" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C266" t="str">
         <f t="shared" si="4"/>
@@ -6056,12 +6065,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:4">
       <c r="A267" t="s">
         <v>278</v>
       </c>
       <c r="B267" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C267" t="str">
         <f t="shared" si="4"/>
@@ -6087,16 +6096,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -6116,23 +6125,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -6143,18 +6152,18 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E4" t="s">
+        <v>424</v>
+      </c>
+      <c r="F4" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
         <v>426</v>
-      </c>
-      <c r="F4" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>428</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -6163,13 +6172,13 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -6191,12 +6200,12 @@
       <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="7" max="7" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -6222,7 +6231,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -6233,18 +6242,18 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F2" t="s">
+        <v>424</v>
+      </c>
+      <c r="G2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
         <v>426</v>
-      </c>
-      <c r="G2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>428</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -6253,13 +6262,13 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F3" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="G3" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>